<commit_message>
Uploaded Excel sheet to a table
</commit_message>
<xml_diff>
--- a/world_population Dashboard.xlsx
+++ b/world_population Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Data Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480C91A4-0B3D-442A-BBB1-40A5A39CE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B06A4CE-9B5C-4A73-A26E-F85A993B4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{8BE078A7-0E5F-4BD6-9F27-81FD0242B2DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BE078A7-0E5F-4BD6-9F27-81FD0242B2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="world_population Working" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -3162,7 +3162,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3205,7 +3205,6 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3252,7 +3251,25 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -3300,7 +3317,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -4719,7 +4736,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable3</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -5396,7 +5413,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable4</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable4</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -6053,7 +6070,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable1</c:name>
     <c:fmtId val="10"/>
   </c:pivotSource>
   <c:chart>
@@ -8368,7 +8385,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable3</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable3</c:name>
     <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
@@ -8523,8 +8540,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -8627,9 +8643,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:xForSave val="1"/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8643,7 +8657,7 @@
         <c:idx val="18"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent2"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -8700,9 +8714,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:xForSave val="1"/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8710,7 +8722,7 @@
         <c:idx val="19"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent3"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -8767,9 +8779,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:xForSave val="1"/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8777,7 +8787,7 @@
         <c:idx val="20"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent4"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -8834,9 +8844,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:xForSave val="1"/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -9445,7 +9453,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[world_population Working.xlsx]Pivot Table!PivotTable4</c:name>
+    <c:name>[world_population Dashboard.xlsx]Pivot Table!PivotTable4</c:name>
     <c:fmtId val="6"/>
   </c:pivotSource>
   <c:chart>
@@ -19599,8 +19607,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Continent 1">
@@ -19623,7 +19631,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -19713,8 +19721,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Continent 2">
@@ -19737,7 +19745,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -20935,8 +20943,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="32" name="Continent 3">
@@ -20959,7 +20967,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -26712,7 +26720,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11BA0B4A-02B7-4547-A27A-36DFE0D19BE7}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11BA0B4A-02B7-4547-A27A-36DFE0D19BE7}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A78:C79" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -27242,7 +27250,7 @@
     <dataField name="Sum of Density (per kmÂ²)" fld="14" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -27251,7 +27259,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -27274,7 +27282,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB1577F-C999-4F7B-9D70-018485E11F58}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB1577F-C999-4F7B-9D70-018485E11F58}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A6:I11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -28144,7 +28152,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0007F16D-66D8-4F33-B694-F15ED57E666F}" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0007F16D-66D8-4F33-B694-F15ED57E666F}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A59:C64" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -28212,7 +28220,7 @@
     <dataField name="Sum of Growth Rate" fld="15" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -28222,7 +28230,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -28284,7 +28292,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A685F31D-72A9-46E0-8D2C-E235F30663A6}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A685F31D-72A9-46E0-8D2C-E235F30663A6}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A40:B45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -28553,6 +28561,35 @@
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="Continent 3" xr10:uid="{988D1244-DBA5-4F71-A273-1240313E4BBD}" cache="Slicer_Continent" caption="Continent" startItem="1" style="SlicerStyleDark5" rowHeight="241300"/>
 </slicers>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE8FDDAB-81F5-41AE-82C9-4FAC13D17F9E}" name="Table1" displayName="Table1" ref="A1:R235" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:R235" xr:uid="{CE8FDDAB-81F5-41AE-82C9-4FAC13D17F9E}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{7CDF05AD-E51B-467B-862A-96DC47CAAD6A}" name="Rank"/>
+    <tableColumn id="2" xr3:uid="{EC4064ED-E016-481A-8154-8FBB3D3BFD2A}" name="CCA3"/>
+    <tableColumn id="3" xr3:uid="{594C3216-0A36-413D-A004-EAD0710D8EA6}" name="Country/Territory"/>
+    <tableColumn id="4" xr3:uid="{F95DB29A-DBB9-4FDC-B931-266CE14486ED}" name="Capital"/>
+    <tableColumn id="5" xr3:uid="{2D740C17-A65C-4A7F-A9D2-3C347CDC5F10}" name="Continent"/>
+    <tableColumn id="6" xr3:uid="{BAF107E0-7470-471E-9B4E-68AFA0E1064F}" name="2022 Population"/>
+    <tableColumn id="7" xr3:uid="{66083E8C-DDAB-486E-8AAD-1F0C541D6A14}" name="2020 Population"/>
+    <tableColumn id="8" xr3:uid="{3CECE118-D1FC-4D63-BBDF-5D85DB573157}" name="2015 Population"/>
+    <tableColumn id="9" xr3:uid="{ED5C439A-4753-4F5D-94D6-7C78F92AB3EE}" name="2010 Population"/>
+    <tableColumn id="10" xr3:uid="{D5859671-D7F4-4122-A567-8B133BF61619}" name="2000 Population"/>
+    <tableColumn id="11" xr3:uid="{9FE2EB26-2AD8-430C-890E-79442D18A568}" name="1990 Population"/>
+    <tableColumn id="12" xr3:uid="{DB856D29-EB77-4120-8123-0CC1CD31BE9E}" name="1980 Population"/>
+    <tableColumn id="13" xr3:uid="{C4712832-A28B-4416-985C-321481BD7C3C}" name="1970 Population"/>
+    <tableColumn id="14" xr3:uid="{2051C95A-FCE2-4D25-9814-4C6EE1B9C510}" name="Area (kmÂ²)"/>
+    <tableColumn id="15" xr3:uid="{8FBA3A0F-C4A2-4F78-AF99-9C66CDDCA924}" name="Density (per kmÂ²)"/>
+    <tableColumn id="16" xr3:uid="{410FA8EC-4D9C-4106-9BBA-92E8F52EDC7B}" name="Growth Rate"/>
+    <tableColumn id="17" xr3:uid="{F70001B4-6B72-427A-A1C8-2CAEBAD3B116}" name="Z-scores of Growth Rate">
+      <calculatedColumnFormula>(P2-$V$26)/$V$27</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{EC8D64A2-4F42-4E4A-B8D1-5A877CFB49E2}" name="World Population Percentage"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28854,28 +28891,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB7379C-0E76-4435-9B55-D238CE1ADBE1}">
   <dimension ref="A1:V235"/>
   <sheetViews>
-    <sheetView topLeftCell="J214" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="7" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" customWidth="1"/>
     <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="24" customWidth="1"/>
-    <col min="18" max="18" width="29" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" customWidth="1"/>
+    <col min="18" max="18" width="29.28515625" customWidth="1"/>
     <col min="20" max="20" width="34" customWidth="1"/>
     <col min="21" max="21" width="22.7109375" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
@@ -42434,6 +42469,9 @@
     <sortCondition descending="1" ref="Q4:Q235"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -42490,28 +42528,28 @@
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7">
         <v>1426730932</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7">
         <v>1360671810</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7">
         <v>1201102442</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7">
         <v>1055228072</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7">
         <v>818946032</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7">
         <v>638150629</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7">
         <v>481536377</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7">
         <v>365444348</v>
       </c>
     </row>
@@ -42519,28 +42557,28 @@
       <c r="A8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8">
         <v>600296136</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8">
         <v>594236593</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8">
         <v>570383850</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8">
         <v>542720651</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8">
         <v>486069584</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8">
         <v>421266425</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8">
         <v>368293361</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8">
         <v>315434606</v>
       </c>
     </row>
@@ -42548,28 +42586,28 @@
       <c r="A9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9">
         <v>45038554</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9">
         <v>43933426</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9">
         <v>40403283</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9">
         <v>37102764</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9">
         <v>31222778</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9">
         <v>26743822</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9">
         <v>22920240</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9">
         <v>19480270</v>
       </c>
     </row>
@@ -42577,28 +42615,28 @@
       <c r="A10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10">
         <v>436816608</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10">
         <v>431530043</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10">
         <v>413134396</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10">
         <v>393078250</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10">
         <v>349634282</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10">
         <v>297146415</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10">
         <v>241789006</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10">
         <v>192947156</v>
       </c>
     </row>
@@ -42606,28 +42644,28 @@
       <c r="A11" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11">
         <v>2508882230</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11">
         <v>2430371872</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11">
         <v>2225023971</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11">
         <v>2028129737</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11">
         <v>1685872676</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11">
         <v>1383307291</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11">
         <v>1114538984</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11">
         <v>893306380</v>
       </c>
     </row>
@@ -42643,7 +42681,7 @@
       <c r="A41" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41">
         <v>30317963</v>
       </c>
     </row>
@@ -42651,7 +42689,7 @@
       <c r="A42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42">
         <v>24244178</v>
       </c>
     </row>
@@ -42659,7 +42697,7 @@
       <c r="A43" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43">
         <v>8515081</v>
       </c>
     </row>
@@ -42667,7 +42705,7 @@
       <c r="A44" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B44">
         <v>17833382</v>
       </c>
     </row>
@@ -42675,7 +42713,7 @@
       <c r="A45" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B45">
         <v>80910604</v>
       </c>
     </row>
@@ -42738,10 +42776,10 @@
       <c r="A64" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="30">
+      <c r="B64">
         <v>21380.284299999999</v>
       </c>
-      <c r="C64" s="30">
+      <c r="C64">
         <v>134.95339999999999</v>
       </c>
     </row>
@@ -42760,7 +42798,7 @@
       <c r="A79" s="9">
         <v>1.0071149253731346</v>
       </c>
-      <c r="B79" s="30">
+      <c r="B79">
         <v>80910604</v>
       </c>
       <c r="C79" s="9">
@@ -42784,7 +42822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446643D-99AE-4FA1-A570-CF4F4838EE3A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>

</xml_diff>